<commit_message>
fix: fixed payload generar schema
</commit_message>
<xml_diff>
--- a/test_documents/Bibliografia.xlsx
+++ b/test_documents/Bibliografia.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{189292AA-E6AB-49C6-8C41-92494BB25E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos actuales\UTP_Experto_Tematico\new_one\interface_et\test_documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803B1A62-C3DB-413C-9870-DDB76A571413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result 1" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -433,7 +436,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,7 +452,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -953,7 +956,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1252,15 +1255,17 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
     <col min="13" max="13" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1342,7 +1347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1456,7 +1461,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1499,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1532,7 +1537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1570,7 +1575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1608,7 +1613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1646,7 +1651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1684,7 +1689,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1727,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1760,7 +1765,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1798,7 +1803,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1836,7 +1841,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1871,7 +1876,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1944,7 +1949,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -1979,7 +1984,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2014,7 +2019,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -2052,7 +2057,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2128,7 +2133,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -2166,7 +2171,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>116</v>
       </c>

</xml_diff>